<commit_message>
Aggiornata checklist con chiarimenti per i casi con ID [32, 40]
GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB-PAINT/1.1.2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB-PAINT/1.1.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111INFOSYSCZ/INFOSYS_SRL/SIOWEB-PAINT/1.1.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\FSE\RSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05576D6C-3FDE-40D1-9A65-A24B9A42C256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D30DC8-7CFB-4F55-A8C3-1EAF5EC523C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4717,9 +4717,6 @@
     <t>Ll'utente viene invitato a riprovare e se il problema persiste di aprire un ticket di supporto sulla piattaforma helpdesk</t>
   </si>
   <si>
-    <t>L'utente viene invitato a riprovare e se il problema persiste di aprire un ticket di supporto sulla piattaforma helpdesk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Viene visualizzato a video un errore di  "Timeout di connessione" e mancata validazione a causa di problemi tecnici. </t>
   </si>
   <si>
@@ -4739,6 +4736,9 @@
   </si>
   <si>
     <t>50d523a9b1a9d847</t>
+  </si>
+  <si>
+    <t>L'utente viene invitato a riprovare e se il problema persiste l'utente medico può in ogni caso proseguire con la produzione e la firma del documento se lo stesso supera con esito positivo la verifica effettuata dal software sulla consistenza e congruità dei dati inseriti, il documento resta nello stato "Da Trasmettere a FSE" e l'utente viene invitato ad aprire un ticket di supporto sulla piattaforma helpdesk. Una volta risolta l'anomalia il documento potrà quindi essere trasmesso a FSE attingendo dalla lista dei documenti non trasmessi.</t>
   </si>
 </sst>
 </file>
@@ -5160,6 +5160,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5181,21 +5196,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7662,7 +7662,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:D2"/>
+      <selection pane="bottomRight" activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -7700,12 +7700,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7723,14 +7723,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="50" t="s">
         <v>848</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="42"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7748,12 +7748,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="50" t="s">
         <v>849</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7772,12 +7772,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50" t="s">
         <v>850</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="42"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7795,8 +7795,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -8899,7 +8899,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="150">
+    <row r="39" spans="1:20" ht="300">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -8918,10 +8918,10 @@
       <c r="F39" s="23">
         <v>45140</v>
       </c>
-      <c r="G39" s="50" t="s">
+      <c r="G39" s="38" t="s">
         <v>912</v>
       </c>
-      <c r="H39" s="50" t="s">
+      <c r="H39" s="38" t="s">
         <v>913</v>
       </c>
       <c r="I39" s="24" t="s">
@@ -8944,7 +8944,7 @@
         <v>137</v>
       </c>
       <c r="P39" s="33" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -9197,7 +9197,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="165">
+    <row r="47" spans="1:20" ht="300">
       <c r="A47" s="20">
         <v>40</v>
       </c>
@@ -9216,11 +9216,11 @@
       <c r="F47" s="23">
         <v>45140</v>
       </c>
-      <c r="G47" s="50" t="s">
+      <c r="G47" s="38" t="s">
+        <v>922</v>
+      </c>
+      <c r="H47" s="38" t="s">
         <v>923</v>
-      </c>
-      <c r="H47" s="50" t="s">
-        <v>924</v>
       </c>
       <c r="I47" s="24" t="s">
         <v>914</v>
@@ -9242,7 +9242,7 @@
         <v>137</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>917</v>
+        <v>924</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -9519,10 +9519,10 @@
       <c r="E55" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="F55" s="48"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="49"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
       <c r="J55" s="33"/>
       <c r="K55" s="33"/>
       <c r="L55" s="33" t="s">
@@ -9532,13 +9532,13 @@
         <v>137</v>
       </c>
       <c r="N55" s="33" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="O55" s="33" t="s">
         <v>137</v>
       </c>
       <c r="P55" s="33" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -12906,13 +12906,13 @@
       <c r="F154" s="23">
         <v>45139</v>
       </c>
-      <c r="G154" s="50" t="s">
+      <c r="G154" s="38" t="s">
         <v>851</v>
       </c>
-      <c r="H154" s="50" t="s">
+      <c r="H154" s="38" t="s">
         <v>852</v>
       </c>
-      <c r="I154" s="50" t="s">
+      <c r="I154" s="38" t="s">
         <v>853</v>
       </c>
       <c r="J154" s="25" t="s">
@@ -13064,13 +13064,13 @@
       <c r="F158" s="23">
         <v>45139</v>
       </c>
-      <c r="G158" s="50" t="s">
+      <c r="G158" s="38" t="s">
         <v>855</v>
       </c>
-      <c r="H158" s="50" t="s">
+      <c r="H158" s="38" t="s">
         <v>856</v>
       </c>
-      <c r="I158" s="50" t="s">
+      <c r="I158" s="38" t="s">
         <v>857</v>
       </c>
       <c r="J158" s="25" t="s">
@@ -13094,7 +13094,7 @@
       </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26"/>
-      <c r="S158" s="46" t="s">
+      <c r="S158" s="34" t="s">
         <v>898</v>
       </c>
       <c r="T158" s="28" t="s">
@@ -13120,13 +13120,13 @@
       <c r="F159" s="23">
         <v>45139</v>
       </c>
-      <c r="G159" s="50" t="s">
+      <c r="G159" s="38" t="s">
         <v>858</v>
       </c>
-      <c r="H159" s="50" t="s">
+      <c r="H159" s="38" t="s">
         <v>859</v>
       </c>
-      <c r="I159" s="50" t="s">
+      <c r="I159" s="38" t="s">
         <v>860</v>
       </c>
       <c r="J159" s="25" t="s">
@@ -13150,7 +13150,7 @@
       </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26"/>
-      <c r="S159" s="46" t="s">
+      <c r="S159" s="34" t="s">
         <v>899</v>
       </c>
       <c r="T159" s="28" t="s">
@@ -13176,13 +13176,13 @@
       <c r="F160" s="23">
         <v>45139</v>
       </c>
-      <c r="G160" s="50" t="s">
+      <c r="G160" s="38" t="s">
         <v>861</v>
       </c>
-      <c r="H160" s="50" t="s">
+      <c r="H160" s="38" t="s">
         <v>862</v>
       </c>
-      <c r="I160" s="50" t="s">
+      <c r="I160" s="38" t="s">
         <v>863</v>
       </c>
       <c r="J160" s="25" t="s">
@@ -13206,7 +13206,7 @@
       </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26"/>
-      <c r="S160" s="46" t="s">
+      <c r="S160" s="34" t="s">
         <v>900</v>
       </c>
       <c r="T160" s="28" t="s">
@@ -13232,13 +13232,13 @@
       <c r="F161" s="23">
         <v>45139</v>
       </c>
-      <c r="G161" s="50" t="s">
+      <c r="G161" s="38" t="s">
         <v>864</v>
       </c>
-      <c r="H161" s="50" t="s">
+      <c r="H161" s="38" t="s">
         <v>865</v>
       </c>
-      <c r="I161" s="50" t="s">
+      <c r="I161" s="38" t="s">
         <v>866</v>
       </c>
       <c r="J161" s="25" t="s">
@@ -13262,7 +13262,7 @@
       </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
-      <c r="S161" s="46" t="s">
+      <c r="S161" s="34" t="s">
         <v>901</v>
       </c>
       <c r="T161" s="28" t="s">
@@ -13288,13 +13288,13 @@
       <c r="F162" s="23">
         <v>45139</v>
       </c>
-      <c r="G162" s="50" t="s">
+      <c r="G162" s="38" t="s">
         <v>867</v>
       </c>
-      <c r="H162" s="50" t="s">
+      <c r="H162" s="38" t="s">
         <v>868</v>
       </c>
-      <c r="I162" s="50" t="s">
+      <c r="I162" s="38" t="s">
         <v>869</v>
       </c>
       <c r="J162" s="25" t="s">
@@ -13318,7 +13318,7 @@
       </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
-      <c r="S162" s="46" t="s">
+      <c r="S162" s="34" t="s">
         <v>902</v>
       </c>
       <c r="T162" s="28" t="s">
@@ -13344,13 +13344,13 @@
       <c r="F163" s="23">
         <v>45139</v>
       </c>
-      <c r="G163" s="50" t="s">
+      <c r="G163" s="38" t="s">
         <v>870</v>
       </c>
-      <c r="H163" s="50" t="s">
+      <c r="H163" s="38" t="s">
         <v>871</v>
       </c>
-      <c r="I163" s="50" t="s">
+      <c r="I163" s="38" t="s">
         <v>872</v>
       </c>
       <c r="J163" s="25" t="s">
@@ -13374,7 +13374,7 @@
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
-      <c r="S163" s="46" t="s">
+      <c r="S163" s="34" t="s">
         <v>903</v>
       </c>
       <c r="T163" s="28" t="s">
@@ -13400,13 +13400,13 @@
       <c r="F164" s="23">
         <v>45139</v>
       </c>
-      <c r="G164" s="50" t="s">
+      <c r="G164" s="38" t="s">
         <v>873</v>
       </c>
-      <c r="H164" s="50" t="s">
+      <c r="H164" s="38" t="s">
         <v>874</v>
       </c>
-      <c r="I164" s="50" t="s">
+      <c r="I164" s="38" t="s">
         <v>875</v>
       </c>
       <c r="J164" s="25" t="s">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="Q164" s="25"/>
       <c r="R164" s="26"/>
-      <c r="S164" s="46" t="s">
+      <c r="S164" s="34" t="s">
         <v>904</v>
       </c>
       <c r="T164" s="28" t="s">
@@ -13456,13 +13456,13 @@
       <c r="F165" s="23">
         <v>45139</v>
       </c>
-      <c r="G165" s="50" t="s">
+      <c r="G165" s="38" t="s">
         <v>876</v>
       </c>
-      <c r="H165" s="50" t="s">
+      <c r="H165" s="38" t="s">
         <v>877</v>
       </c>
-      <c r="I165" s="50" t="s">
+      <c r="I165" s="38" t="s">
         <v>878</v>
       </c>
       <c r="J165" s="25" t="s">
@@ -13486,7 +13486,7 @@
       </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26"/>
-      <c r="S165" s="46" t="s">
+      <c r="S165" s="34" t="s">
         <v>905</v>
       </c>
       <c r="T165" s="28" t="s">
@@ -13512,13 +13512,13 @@
       <c r="F166" s="23">
         <v>45139</v>
       </c>
-      <c r="G166" s="50" t="s">
+      <c r="G166" s="38" t="s">
         <v>879</v>
       </c>
-      <c r="H166" s="50" t="s">
+      <c r="H166" s="38" t="s">
         <v>880</v>
       </c>
-      <c r="I166" s="50" t="s">
+      <c r="I166" s="38" t="s">
         <v>881</v>
       </c>
       <c r="J166" s="25" t="s">
@@ -13542,7 +13542,7 @@
       </c>
       <c r="Q166" s="25"/>
       <c r="R166" s="26"/>
-      <c r="S166" s="46" t="s">
+      <c r="S166" s="34" t="s">
         <v>906</v>
       </c>
       <c r="T166" s="28" t="s">
@@ -13568,13 +13568,13 @@
       <c r="F167" s="23">
         <v>45139</v>
       </c>
-      <c r="G167" s="50" t="s">
+      <c r="G167" s="38" t="s">
         <v>882</v>
       </c>
-      <c r="H167" s="50" t="s">
+      <c r="H167" s="38" t="s">
         <v>883</v>
       </c>
-      <c r="I167" s="50" t="s">
+      <c r="I167" s="38" t="s">
         <v>884</v>
       </c>
       <c r="J167" s="25" t="s">
@@ -13598,7 +13598,7 @@
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
-      <c r="S167" s="46" t="s">
+      <c r="S167" s="34" t="s">
         <v>907</v>
       </c>
       <c r="T167" s="28" t="s">
@@ -13624,13 +13624,13 @@
       <c r="F168" s="23">
         <v>45139</v>
       </c>
-      <c r="G168" s="50" t="s">
+      <c r="G168" s="38" t="s">
         <v>885</v>
       </c>
-      <c r="H168" s="50" t="s">
+      <c r="H168" s="38" t="s">
         <v>886</v>
       </c>
-      <c r="I168" s="50" t="s">
+      <c r="I168" s="38" t="s">
         <v>887</v>
       </c>
       <c r="J168" s="25" t="s">
@@ -13654,7 +13654,7 @@
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
-      <c r="S168" s="46" t="s">
+      <c r="S168" s="34" t="s">
         <v>908</v>
       </c>
       <c r="T168" s="28" t="s">
@@ -13694,7 +13694,7 @@
       <c r="P169" s="25"/>
       <c r="Q169" s="25"/>
       <c r="R169" s="26"/>
-      <c r="S169" s="47"/>
+      <c r="S169" s="35"/>
       <c r="T169" s="28" t="s">
         <v>103</v>
       </c>
@@ -13718,13 +13718,13 @@
       <c r="F170" s="23">
         <v>45139</v>
       </c>
-      <c r="G170" s="50" t="s">
+      <c r="G170" s="38" t="s">
         <v>891</v>
       </c>
-      <c r="H170" s="50" t="s">
+      <c r="H170" s="38" t="s">
         <v>892</v>
       </c>
-      <c r="I170" s="50" t="s">
+      <c r="I170" s="38" t="s">
         <v>893</v>
       </c>
       <c r="J170" s="25" t="s">
@@ -13748,7 +13748,7 @@
       </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26"/>
-      <c r="S170" s="46" t="s">
+      <c r="S170" s="34" t="s">
         <v>909</v>
       </c>
       <c r="T170" s="28" t="s">
@@ -13788,7 +13788,7 @@
       <c r="P171" s="25"/>
       <c r="Q171" s="25"/>
       <c r="R171" s="26"/>
-      <c r="S171" s="47"/>
+      <c r="S171" s="35"/>
       <c r="T171" s="28" t="s">
         <v>103</v>
       </c>
@@ -13826,7 +13826,7 @@
       <c r="P172" s="25"/>
       <c r="Q172" s="25"/>
       <c r="R172" s="26"/>
-      <c r="S172" s="47"/>
+      <c r="S172" s="35"/>
       <c r="T172" s="28" t="s">
         <v>103</v>
       </c>
@@ -13864,7 +13864,7 @@
       <c r="P173" s="25"/>
       <c r="Q173" s="25"/>
       <c r="R173" s="26"/>
-      <c r="S173" s="47"/>
+      <c r="S173" s="35"/>
       <c r="T173" s="28" t="s">
         <v>103</v>
       </c>
@@ -13902,7 +13902,7 @@
       <c r="P174" s="25"/>
       <c r="Q174" s="25"/>
       <c r="R174" s="26"/>
-      <c r="S174" s="47"/>
+      <c r="S174" s="35"/>
       <c r="T174" s="28" t="s">
         <v>103</v>
       </c>
@@ -13940,7 +13940,7 @@
       <c r="P175" s="25"/>
       <c r="Q175" s="25"/>
       <c r="R175" s="26"/>
-      <c r="S175" s="47"/>
+      <c r="S175" s="35"/>
       <c r="T175" s="28" t="s">
         <v>103</v>
       </c>
@@ -13964,13 +13964,13 @@
       <c r="F176" s="23">
         <v>45139</v>
       </c>
-      <c r="G176" s="50" t="s">
+      <c r="G176" s="38" t="s">
         <v>894</v>
       </c>
-      <c r="H176" s="50" t="s">
+      <c r="H176" s="38" t="s">
         <v>895</v>
       </c>
-      <c r="I176" s="50" t="s">
+      <c r="I176" s="38" t="s">
         <v>896</v>
       </c>
       <c r="J176" s="25" t="s">
@@ -13994,7 +13994,7 @@
       </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26"/>
-      <c r="S176" s="46" t="s">
+      <c r="S176" s="34" t="s">
         <v>911</v>
       </c>
       <c r="T176" s="28" t="s">
@@ -20956,14 +20956,14 @@
       <c r="F381" s="23">
         <v>45140</v>
       </c>
-      <c r="G381" s="50" t="s">
+      <c r="G381" s="38" t="s">
+        <v>919</v>
+      </c>
+      <c r="H381" s="38" t="s">
         <v>920</v>
       </c>
-      <c r="H381" s="50" t="s">
+      <c r="I381" s="38" t="s">
         <v>921</v>
-      </c>
-      <c r="I381" s="50" t="s">
-        <v>922</v>
       </c>
       <c r="J381" s="33" t="s">
         <v>137</v>
@@ -20976,7 +20976,7 @@
       <c r="P381" s="25"/>
       <c r="Q381" s="25"/>
       <c r="R381" s="26"/>
-      <c r="S381" s="47"/>
+      <c r="S381" s="35"/>
       <c r="T381" s="28" t="s">
         <v>47</v>
       </c>

</xml_diff>